<commit_message>
Added conditioned coloring for comparison file
</commit_message>
<xml_diff>
--- a/analysis/20-08-2018 - tmp - table4michal.xlsx
+++ b/analysis/20-08-2018 - tmp - table4michal.xlsx
@@ -55,6 +55,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,9 +95,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -397,7 +401,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H2" sqref="H2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -452,16 +456,16 @@
       <c r="C2" s="1">
         <v>0.3</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>20.469804878048802</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>68.232682926829199</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>0.77341463414634104</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>2.5468292682926799</v>
       </c>
       <c r="H2" s="2">
@@ -484,25 +488,25 @@
       <c r="C3" s="1">
         <v>0.5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>34.116341463414599</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>68.232682926829199</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>0.77341463414634104</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="4">
         <v>2.5468292682926799</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>0.98071881606765399</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
         <v>0.95819238900634096</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="3">
         <v>0.97266384778012704</v>
       </c>
     </row>
@@ -516,25 +520,25 @@
       <c r="C4" s="1">
         <v>0.3</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>22.922634146341501</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>76.408780487804904</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>0.88390243902439003</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="4">
         <v>2.7678048780487798</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>0.99599365750528002</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="3">
         <v>0.98067653276955502</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="3">
         <v>0.99754756871035899</v>
       </c>
     </row>
@@ -548,25 +552,25 @@
       <c r="C5" s="1">
         <v>0.5</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>38.204390243902402</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>76.408780487804904</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <v>0.88390243902439003</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="4">
         <v>2.7678048780487798</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>0.99599365750528002</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>0.99236786469344496</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="3">
         <v>0.99754756871035899</v>
       </c>
     </row>
@@ -580,25 +584,25 @@
       <c r="C6" s="1">
         <v>0.3</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>80.552653846153802</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>268.50884615384598</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>1.6701282051282</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="4">
         <v>4.3402564102564103</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>0.944536296770075</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
         <v>0.92444515510073499</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3">
         <v>0.75511832427246495</v>
       </c>
     </row>
@@ -612,25 +616,25 @@
       <c r="C7" s="1">
         <v>0.5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>134.25442307692299</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>268.50884615384598</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <v>1.6701282051282</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="4">
         <v>4.3402564102564103</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>0.944536296770075</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <v>0.95475695554844897</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="3">
         <v>0.71689958426607003</v>
       </c>
     </row>
@@ -644,25 +648,25 @@
       <c r="C8" s="1">
         <v>0.3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>91.074461538461506</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <v>303.58153846153903</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>1.90871794871795</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="4">
         <v>4.8174358974359004</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>0.97289734569875796</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
         <v>0.97785577230572396</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="3">
         <v>0.827785417332907</v>
       </c>
     </row>
@@ -676,25 +680,25 @@
       <c r="C9" s="1">
         <v>0.5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>151.790769230769</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="4">
         <v>303.58153846153903</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="4">
         <v>1.90871794871795</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="4">
         <v>4.8174358974359004</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>0.97289734569875796</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <v>0.97410297409657798</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="3">
         <v>0.94183242724656202</v>
       </c>
     </row>
@@ -708,25 +712,25 @@
       <c r="C10" s="1">
         <v>0.3</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <v>515.94216201117297</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <v>1719.80720670391</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="4">
         <v>3.52013966480447</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="4">
         <v>17.0402793296089</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <v>0.47685054219707901</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
         <v>0.754559170202734</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="3">
         <v>0.39906176331918902</v>
       </c>
     </row>
@@ -740,25 +744,25 @@
       <c r="C11" s="1">
         <v>0.5</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="4">
         <v>859.90360335195498</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>1719.80720670391</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <v>3.52013966480447</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="4">
         <v>17.0402793296089</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <v>0.46425271098538601</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
         <v>0.76085808580858105</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="3">
         <v>0.43403583215464397</v>
       </c>
     </row>
@@ -772,25 +776,25 @@
       <c r="C12" s="1">
         <v>0.3</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="4">
         <v>566.93389944134105</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>1889.77966480447</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="4">
         <v>4.0230167597765396</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="4">
         <v>18.046033519553099</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <v>0.63668552569542802</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="3">
         <v>0.79044318717586004</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="3">
         <v>0.55479962281942496</v>
       </c>
     </row>
@@ -804,25 +808,25 @@
       <c r="C13" s="1">
         <v>0.5</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="4">
         <v>944.88983240223502</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <v>1889.77966480447</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="4">
         <v>4.0230167597765396</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="4">
         <v>18.046033519553099</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="3">
         <v>0.62598774163130699</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3">
         <v>0.86353606789250403</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="3">
         <v>0.69792079207920799</v>
       </c>
     </row>
@@ -836,23 +840,23 @@
       <c r="C14" s="1">
         <v>0.3</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="4">
         <v>2693.8820904645499</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4">
         <v>8979.6069682151792</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="4">
         <v>10.012396088019599</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="4">
         <v>30.024792176039099</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3">
         <v>0.73198667373934101</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="3">
         <v>0.61192849609919597</v>
       </c>
     </row>
@@ -866,23 +870,23 @@
       <c r="C15" s="1">
         <v>0.5</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="4">
         <v>4489.8034841075796</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <v>8979.6069682151792</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="4">
         <v>10.012396088019599</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="4">
         <v>30.024792176039099</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3">
         <v>0.77868595857453504</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="3">
         <v>0.66409704939480396</v>
       </c>
     </row>
@@ -896,23 +900,23 @@
       <c r="C16" s="1">
         <v>0.3</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="4">
         <v>3026.4366748166299</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="4">
         <v>10088.1222493888</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="4">
         <v>11.4427383863081</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="4">
         <v>32.885476772616101</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3">
         <v>0.81518428859866698</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="3">
         <v>0.71970177355001397</v>
       </c>
     </row>
@@ -926,208 +930,208 @@
       <c r="C17" s="1">
         <v>0.5</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="4">
         <v>5044.0611246943799</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
         <v>10088.1222493888</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="4">
         <v>11.4427383863081</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="4">
         <v>32.885476772616101</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3">
         <v>0.93677676416753797</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="3">
         <v>0.937098363989744</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H3:J3">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:J4">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:J5">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:J6">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:J7">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:J8">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:J9">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:J10">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11:J11">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:J12">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:J13">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:J14">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:J15">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:J16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:J17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H2:J2">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:J3">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:J4">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5:J5">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:J6">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:J7">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8:J8">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9:J9">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10:J10">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H11:J11">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12:J12">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13:J13">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14:J14">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:J15">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:J16">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17:J17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Updated results for LNS after bug fix
</commit_message>
<xml_diff>
--- a/analysis/20-08-2018 - tmp - table4michal.xlsx
+++ b/analysis/20-08-2018 - tmp - table4michal.xlsx
@@ -401,7 +401,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:J2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -471,8 +471,8 @@
       <c r="H2" s="2">
         <v>0.98071881606765399</v>
       </c>
-      <c r="I2" s="2">
-        <v>0.965031712473573</v>
+      <c r="I2" s="3">
+        <v>0.98071881606765199</v>
       </c>
       <c r="J2" s="2">
         <v>0.94982029598308704</v>
@@ -504,7 +504,7 @@
         <v>0.98071881606765399</v>
       </c>
       <c r="I3" s="3">
-        <v>0.95819238900634096</v>
+        <v>0.98071881606765199</v>
       </c>
       <c r="J3" s="3">
         <v>0.97266384778012704</v>
@@ -536,7 +536,7 @@
         <v>0.99599365750528002</v>
       </c>
       <c r="I4" s="3">
-        <v>0.98067653276955502</v>
+        <v>0.99076109936574897</v>
       </c>
       <c r="J4" s="3">
         <v>0.99754756871035899</v>
@@ -568,7 +568,7 @@
         <v>0.99599365750528002</v>
       </c>
       <c r="I5" s="3">
-        <v>0.99236786469344496</v>
+        <v>0.99298097251585504</v>
       </c>
       <c r="J5" s="3">
         <v>0.99754756871035899</v>
@@ -600,7 +600,7 @@
         <v>0.944536296770075</v>
       </c>
       <c r="I6" s="3">
-        <v>0.92444515510073499</v>
+        <v>0.947779021426287</v>
       </c>
       <c r="J6" s="3">
         <v>0.75511832427246495</v>
@@ -632,7 +632,7 @@
         <v>0.944536296770075</v>
       </c>
       <c r="I7" s="3">
-        <v>0.95475695554844897</v>
+        <v>0.97173968660057497</v>
       </c>
       <c r="J7" s="3">
         <v>0.71689958426607003</v>
@@ -664,7 +664,7 @@
         <v>0.97289734569875796</v>
       </c>
       <c r="I8" s="3">
-        <v>0.97785577230572396</v>
+        <v>0.97804285257435197</v>
       </c>
       <c r="J8" s="3">
         <v>0.827785417332907</v>
@@ -696,7 +696,7 @@
         <v>0.97289734569875796</v>
       </c>
       <c r="I9" s="3">
-        <v>0.97410297409657798</v>
+        <v>0.98357211384713805</v>
       </c>
       <c r="J9" s="3">
         <v>0.94183242724656202</v>
@@ -728,7 +728,7 @@
         <v>0.47685054219707901</v>
       </c>
       <c r="I10" s="3">
-        <v>0.754559170202734</v>
+        <v>0.72402640264026397</v>
       </c>
       <c r="J10" s="3">
         <v>0.39906176331918902</v>
@@ -760,7 +760,7 @@
         <v>0.46425271098538601</v>
       </c>
       <c r="I11" s="3">
-        <v>0.76085808580858105</v>
+        <v>0.71724186704384696</v>
       </c>
       <c r="J11" s="3">
         <v>0.43403583215464397</v>
@@ -792,7 +792,7 @@
         <v>0.63668552569542802</v>
       </c>
       <c r="I12" s="3">
-        <v>0.79044318717586004</v>
+        <v>0.829434229137199</v>
       </c>
       <c r="J12" s="3">
         <v>0.55479962281942496</v>
@@ -824,7 +824,7 @@
         <v>0.62598774163130699</v>
       </c>
       <c r="I13" s="3">
-        <v>0.86353606789250403</v>
+        <v>0.86489391796322501</v>
       </c>
       <c r="J13" s="3">
         <v>0.69792079207920799</v>
@@ -854,7 +854,7 @@
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3">
-        <v>0.73198667373934101</v>
+        <v>0.71525763754499905</v>
       </c>
       <c r="J14" s="3">
         <v>0.61192849609919597</v>
@@ -884,7 +884,7 @@
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3">
-        <v>0.77868595857453504</v>
+        <v>0.78692712279826305</v>
       </c>
       <c r="J15" s="3">
         <v>0.66409704939480396</v>
@@ -914,7 +914,7 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3">
-        <v>0.81518428859866698</v>
+        <v>0.85457085289326196</v>
       </c>
       <c r="J16" s="3">
         <v>0.71970177355001397</v>
@@ -944,7 +944,7 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3">
-        <v>0.93677676416753797</v>
+        <v>0.87163815302556102</v>
       </c>
       <c r="J17" s="3">
         <v>0.937098363989744</v>

</xml_diff>